<commit_message>
fight with migrations and context
</commit_message>
<xml_diff>
--- a/OuterData/checklist.xlsx
+++ b/OuterData/checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218CD7CF-1CE2-4057-9364-5757119BD9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC380CD-3C35-4E70-8B4F-426D8B5C6364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>db structure</t>
   </si>
@@ -40,10 +40,16 @@
     <t>why use application user instead of identityuser</t>
   </si>
   <si>
-    <t>return purchase</t>
-  </si>
-  <si>
     <t>reserved sale, so that sale could have a statuses like "sold" "reserved" "returned"</t>
+  </si>
+  <si>
+    <t>purchase return</t>
+  </si>
+  <si>
+    <t>how to bind IdentityRole(s) with real mysql roles? (probably it's so hard to implement)</t>
+  </si>
+  <si>
+    <t>do i need it on the whole? all queries are server-side.</t>
   </si>
 </sst>
 </file>
@@ -361,55 +367,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="88" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
did in college (so little)
</commit_message>
<xml_diff>
--- a/OuterData/checklist.xlsx
+++ b/OuterData/checklist.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B2ED8D-5397-4032-8E8C-E57DEF66FDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -55,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -65,12 +64,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -85,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -366,11 +372,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,7 +386,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -390,7 +396,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -400,7 +406,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -429,5 +435,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
i like the way goods search works now
</commit_message>
<xml_diff>
--- a/OuterData/checklist.xlsx
+++ b/OuterData/checklist.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F77CD1-EE71-4494-9705-558155799048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>db structure</t>
   </si>
@@ -49,12 +50,18 @@
   </si>
   <si>
     <t>do i need it on the whole? all queries are server-side.</t>
+  </si>
+  <si>
+    <t>&amp;__Invariant when using asp-for=""</t>
+  </si>
+  <si>
+    <t>why pass data using ViewBag instead of passing model?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -372,11 +379,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,6 +440,16 @@
         <v>9</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
what did i want to do?
</commit_message>
<xml_diff>
--- a/OuterData/checklist.xlsx
+++ b/OuterData/checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50821EE-5397-40F5-97FE-EB00A3575896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2E6DF1-E93D-4DBE-A3FE-8EB47E41ABDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>db structure</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>bind sales_view to sales and to ef core</t>
+  </si>
+  <si>
+    <t>Guid in ef core</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,6 +539,11 @@
         <v>20</v>
       </c>
     </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
it's bad when you write code for 3 hours and don't run the program even once
</commit_message>
<xml_diff>
--- a/OuterData/checklist.xlsx
+++ b/OuterData/checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30372F8-8E77-4757-B134-BC86EF78F656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6FE9A0-B14A-445D-B72B-527EE573BDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>db structure</t>
   </si>
@@ -97,7 +97,16 @@
     <t>when to call dto and when to call model</t>
   </si>
   <si>
-    <t>html and DRY principle?? (in its defense i'll say that html is not a programming language at least)</t>
+    <t>html and DRY principle?? (in its defense i'll say that html is not a programming language after all)</t>
+  </si>
+  <si>
+    <t>how to edit log in page</t>
+  </si>
+  <si>
+    <t>don't like async everywhere in service layer</t>
+  </si>
+  <si>
+    <t>[.. ]</t>
   </si>
 </sst>
 </file>
@@ -436,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,13 +576,28 @@
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pilka, los, kwiat, etc. polish stuff.
</commit_message>
<xml_diff>
--- a/OuterData/checklist.xlsx
+++ b/OuterData/checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29700080-C18D-4B05-BAFC-856D58E6FB36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E014AB32-2466-4592-AA2B-411FFA9DE5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>db structure</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>factory for goods creating</t>
+  </si>
+  <si>
+    <t>use correct verb for each request</t>
   </si>
 </sst>
 </file>
@@ -472,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,6 +675,11 @@
         <v>37</v>
       </c>
     </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
backups stuff! i spent approx 2.5 hours to make "mysqldump" working. "ProcessStartInfo" is so insidious class.
</commit_message>
<xml_diff>
--- a/OuterData/checklist.xlsx
+++ b/OuterData/checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84C9591-D564-433E-B9E1-08C54B2DF68D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84CE1ED-6381-4DB0-A0FB-56E62AE124F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>db structure</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>validation IN PARTICULARLY, VALIDATE THAT FIELDS DON'T CONTAINT HTML TAGS</t>
+  </si>
+  <si>
+    <t>when to use GET and POST in form when you send no data but this request updates the state of application (actually, not of application but of server file system. it creates some files, not related to db directly)</t>
   </si>
 </sst>
 </file>
@@ -199,11 +202,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -484,15 +496,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="135.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="135.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -502,7 +514,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -512,7 +524,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -522,22 +534,22 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -545,7 +557,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -560,12 +572,12 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -575,22 +587,22 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -600,17 +612,17 @@
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -620,88 +632,93 @@
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="2" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="2" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
model validation: wait, i'm coming
</commit_message>
<xml_diff>
--- a/OuterData/checklist.xlsx
+++ b/OuterData/checklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1D37CF-41F1-4E52-8209-9D236F924BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFFAB77-1AD3-46D3-BEAA-53E7C7DA5696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>db structure</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>if database is corrupted, then send admin immediately to backups</t>
+  </si>
+  <si>
+    <t>strange tiny shift like Год выпуска [___] and Год выпуска   [___] In addGoodsToWarehouse</t>
+  </si>
+  <si>
+    <t>sort specific types</t>
   </si>
 </sst>
 </file>
@@ -517,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,6 +768,16 @@
         <v>46</v>
       </c>
     </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>